<commit_message>
Can add up to 200 work orders to the table
</commit_message>
<xml_diff>
--- a/src/Files/InventoryWorkbookTest.xlsx
+++ b/src/Files/InventoryWorkbookTest.xlsx
@@ -4,27 +4,56 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="InventorySheet" sheetId="1" r:id="rId1"/>
     <sheet name="TestSheet1" sheetId="2" r:id="rId2"/>
     <sheet name="TestSheet2" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="A13" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This is a comment
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>inventory work book</t>
-  </si>
-  <si>
-    <t>qty</t>
-  </si>
-  <si>
-    <t>PART #</t>
   </si>
   <si>
     <t>This sheet is a test</t>
@@ -33,17 +62,26 @@
     <t xml:space="preserve">This sheet is also a test </t>
   </si>
   <si>
-    <t>Qty Needed</t>
+    <t>Part #</t>
   </si>
   <si>
-    <t>What should be left</t>
+    <t xml:space="preserve">Qty </t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>1ft</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,19 +91,78 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -73,50 +170,21 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,201 +486,207 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1">
-        <v>5200</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="1">
-        <v>5202</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="3">
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>23</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14">
+        <v>45</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="1">
-        <v>5349</v>
-      </c>
-      <c r="B5">
-        <v>2</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="3">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="1">
-        <v>5352</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="3">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="1">
-        <v>6244</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="4">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="1">
-        <v>6245</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="4">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="1">
-        <v>6431</v>
-      </c>
-      <c r="B9">
-        <v>22</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="4">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="1">
-        <v>6434</v>
-      </c>
-      <c r="B10">
-        <v>96</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="4">
-        <v>2</v>
-      </c>
-      <c r="F10">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="1">
-        <v>6466</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="1">
-        <v>6546</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="1">
-        <v>6588</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f>SUM(A3:A4)</f>
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -624,11 +698,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -644,11 +718,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>